<commit_message>
adding data for HPC
</commit_message>
<xml_diff>
--- a/output/countAllData.xlsx
+++ b/output/countAllData.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -397,17 +397,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>70423</t>
+          <t>80526</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>336</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>680</t>
+          <t>689</t>
         </is>
       </c>
     </row>
@@ -424,17 +424,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11264</t>
+          <t>11146</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>68</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>123</t>
         </is>
       </c>
     </row>
@@ -451,17 +451,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>24485</t>
+          <t>26228</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>154</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>348</t>
         </is>
       </c>
     </row>
@@ -478,17 +478,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>28996</t>
+          <t>35957</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>200</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>344</t>
+          <t>369</t>
         </is>
       </c>
     </row>
@@ -505,17 +505,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11913</t>
+          <t>11774</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>59</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>114</t>
         </is>
       </c>
     </row>
@@ -559,44 +559,71 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>6842</t>
+          <t>6818</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>79</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>132</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>PRMDN</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>plantasMortas</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>7740</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>156562</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>657</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1801</t>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>182828</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>963</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1876</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionei linha que remove check do COSTR
</commit_message>
<xml_diff>
--- a/output/countAllData.xlsx
+++ b/output/countAllData.xlsx
@@ -397,17 +397,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>80526</t>
+          <t>82132</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>336</t>
+          <t>343</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>689</t>
+          <t>701</t>
         </is>
       </c>
     </row>
@@ -424,17 +424,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11146</t>
+          <t>11149</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>69</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>124</t>
         </is>
       </c>
     </row>
@@ -451,17 +451,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>26228</t>
+          <t>26374</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>157</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>351</t>
         </is>
       </c>
     </row>
@@ -478,17 +478,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>35957</t>
+          <t>36752</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>205</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>369</t>
+          <t>376</t>
         </is>
       </c>
     </row>
@@ -505,17 +505,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11774</t>
+          <t>12620</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>64</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>121</t>
         </is>
       </c>
     </row>
@@ -559,17 +559,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>6818</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>80</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>133</t>
         </is>
       </c>
     </row>
@@ -586,17 +586,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7740</t>
+          <t>8914</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>42</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>76</t>
         </is>
       </c>
     </row>
@@ -613,17 +613,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>182828</t>
+          <t>187640</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>963</t>
+          <t>995</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1876</t>
+          <t>1920</t>
         </is>
       </c>
     </row>

</xml_diff>